<commit_message>
Refactor: Admin Interests Dashboard redesign, Modal refinements, and Interest Withdrawal workflow optimizations.
- Redesigned Admin Interests Dashboard with summary stats bar and enlarged, better-separated data table.
- Refined 'Show Interest' modal with italicized checkbox labels for professional appearance.
- Simplified Interest Withdrawal flow on localhost (removed email prompt).
- Fixed bug where 'My Interests' list appeared empty due to data structure mismatch.
- Added multi-language support for new withdrawal features.
</commit_message>
<xml_diff>
--- a/storage/UserInterests.xlsx
+++ b/storage/UserInterests.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,16 @@
           <t>Timestamp</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Event Price Amount</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Event Price Currency</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -536,6 +546,8 @@
           <t>2026-01-05 13:44:50</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -588,6 +600,8 @@
           <t>2026-01-05 13:52:05</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -640,6 +654,8 @@
           <t>2026-01-05 13:57:11</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -692,6 +708,8 @@
           <t>2026-01-05 21:02:48</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -744,6 +762,8 @@
           <t>2026-01-05 21:19:21</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -796,6 +816,8 @@
           <t>2026-01-05 21:19:53</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -848,6 +870,8 @@
           <t>2026-01-05 21:20:43</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -900,6 +924,8 @@
           <t>2026-01-05 21:29:54</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -952,6 +978,8 @@
           <t>2026-01-05 21:30:24</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1004,6 +1032,8 @@
           <t>2026-01-05 21:31:37</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1056,6 +1086,8 @@
           <t>2026-01-05 21:32:59</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1108,6 +1140,224 @@
           <t>2026-01-05 21:55:59</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>shiv</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sawale</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sawashi01</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Shivam.Sawale@bakerhughes.com</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Intern</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>hyderabad</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>The Energy Summit / Future Energy Meet 2026</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2026-01-06 14:14:34</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>shiv</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>sawale</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>sawashi01</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Shivam.Sawale@bakerhughes.com</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Intern</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>hyderabad</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>World Conf. on Robotics and Automation</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>2026-01-06 14:18:46</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>shiv</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sawale</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>sawashi01</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Shivam.Sawale@bakerhughes.com</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Intern</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>hyderabad</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>The 11th Asia-Pacific Optical Sensors Conference (APOS),</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2026-01-06 14:22:33</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>shiv</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sawale</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sawashi01</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Shivam.Sawale@bakerhughes.com</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Intern</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>hyderabad</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Gartner Security &amp; Risk Management Summit 2026 (US)</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>2026-01-06 14:42:04</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>